<commit_message>
Adding column ('CLAVE DE LA ENTIDAD') to datosPoblacion.xlsx
</commit_message>
<xml_diff>
--- a/datosModificados/datosPoblacion.xlsx
+++ b/datosModificados/datosPoblacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,837 +436,938 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>CLAVE DE LA ENTIDAD</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Entidad federativa</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>PoblacionTotal2010</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Poblacion10a14-2010</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Poblacion15a19-2010</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>PoblacionTotal2020</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Poblacion10a14-2020</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Poblacion15a19-2020</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Aguascalientes</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>1184996</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>123806</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>121428</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1425607</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>129717</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>131967</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Baja California</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>3155070</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>305472</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>299195</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>3769020</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>312348</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>315639</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Baja California Sur</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>637026</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>57380</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>57713</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>798447</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>67665</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>65469</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Campeche</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>822441</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>81314</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>82920</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>928363</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>80168</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>76140</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Coahuila de Zaragoza</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>2748391</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>268193</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>261942</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>3146771</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>268144</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>269284</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Colima</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>650555</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>59473</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>62323</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>731391</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>60801</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>60663</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Chiapas</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>4796580</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>549896</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>530233</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>5543828</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>583132</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>526577</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Chihuahua</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>3406465</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>324661</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>322034</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>3741869</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>333715</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>326333</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Ciudad de México</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>8851080</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>660345</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>723372</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>9209944</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>608962</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>650389</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Durango</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>1632934</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>167180</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>166366</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>1832650</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>170271</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>162990</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Guanajuato</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>5486372</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>580600</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>570965</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>6166934</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>549301</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>552092</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Guerrero</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>3388768</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>393378</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>372191</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>3540685</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>348493</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>326540</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Hidalgo</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>2665018</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>263026</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>269602</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>3082841</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>283676</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>272506</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Jalisco</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>7350682</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>714393</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>715003</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>8348151</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>714906</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>716259</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>México</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>15175862</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>1429028</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>1467148</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>16992418</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>1464549</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>1476665</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Michoacán de Ocampo</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="C17" t="n">
         <v>4351037</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>443721</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>453827</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>4748846</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>426869</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>407743</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Morelos</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="C18" t="n">
         <v>1777227</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>167487</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>175625</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>1971520</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>164177</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>166654</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Nayarit</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="C19" t="n">
         <v>1084979</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>104308</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>107191</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>1235456</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>113335</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>104256</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Nuevo León</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="C20" t="n">
         <v>4653458</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>415368</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>406428</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>5784442</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>462720</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>471896</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>Oaxaca</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="C21" t="n">
         <v>3801962</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>414392</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>406873</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>4132148</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>398362</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>358708</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>Puebla</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="C22" t="n">
         <v>5779829</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>604845</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>604094</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>6583278</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>603375</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>607200</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>Querétaro</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="C23" t="n">
         <v>1827937</v>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>182608</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>187241</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>2368467</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>198601</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>198141</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>Quintana Roo</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="C24" t="n">
         <v>1325578</v>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>121308</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>128650</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>1857985</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>154281</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>147549</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>San Luis Potosí</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="C25" t="n">
         <v>2585518</v>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>270154</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>269673</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>2822255</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>252780</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>253797</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Sinaloa</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="C26" t="n">
         <v>2767761</v>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>270555</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>275540</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>3026943</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>260172</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>261581</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>Sonora</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="C27" t="n">
         <v>2662480</v>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>256883</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>251510</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>2944840</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>258791</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>255716</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>Tabasco</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="C28" t="n">
         <v>2238603</v>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="n">
         <v>220776</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>224257</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>2402598</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>222698</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>208660</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Tamaulipas</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="C29" t="n">
         <v>3268554</v>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>294469</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>291682</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>3527735</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>305853</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>294950</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>Tlaxcala</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="C30" t="n">
         <v>1169936</v>
       </c>
-      <c r="C30" t="n">
+      <c r="D30" t="n">
         <v>118634</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>119172</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>1342977</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>119718</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>121207</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>Veracruz de Ignacio de la Llave</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="C31" t="n">
         <v>7643194</v>
       </c>
-      <c r="C31" t="n">
+      <c r="D31" t="n">
         <v>741526</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>759388</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>8062579</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>685468</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>681548</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>Yucatán</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="C32" t="n">
         <v>1955577</v>
       </c>
-      <c r="C32" t="n">
+      <c r="D32" t="n">
         <v>182604</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>192027</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>2320898</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>189137</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>196363</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Zacatecas</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="C33" t="n">
         <v>1490668</v>
       </c>
-      <c r="C33" t="n">
+      <c r="D33" t="n">
         <v>152154</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>150499</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>1622138</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>151355</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>141208</v>
       </c>
     </row>

</xml_diff>